<commit_message>
el 28 como pide
</commit_message>
<xml_diff>
--- a/informe/public/presupuesto.xlsx
+++ b/informe/public/presupuesto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MARROQUIN\Desktop\-ORGA-Proyecto_G3\informe\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDB0A6F-AD18-4197-99BA-346FED44AC38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F797902C-DD00-4479-9979-1A06142406EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="28" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="28" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -601,7 +601,9 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
+      <c r="A2" s="12">
+        <v>45770</v>
+      </c>
       <c r="B2" s="4"/>
       <c r="C2" s="10"/>
     </row>

</xml_diff>